<commit_message>
Ajuste Observaciones Cotización Modulo Solicitante Ver Update
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Selección para carga de tipo Bien</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>DESCRIPCIÓN SERVICIO 2</t>
+  </si>
+  <si>
+    <t>0 - NO APLICA</t>
   </si>
 </sst>
 </file>
@@ -365,21 +368,20 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,22 +485,21 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.2091836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6683673469388"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.3673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,7 +577,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E4" s="9" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Ajuste Modulo Gestion Cotizaciones, Solicitud Modificar, Vista Adendas
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Selección para carga de tipo Bien</t>
   </si>
@@ -86,33 +86,9 @@
     <t>Campo para descripcion del Servicio</t>
   </si>
   <si>
-    <t>Campo selección para unidad  del Servicio</t>
-  </si>
-  <si>
-    <t>Cantidad en años para T.E.</t>
-  </si>
-  <si>
-    <t>Cantidad en meses para T.E.</t>
-  </si>
-  <si>
-    <t>Cantidad en días  para T.E.</t>
-  </si>
-  <si>
     <t>Campo para cantidad  del Servicio</t>
   </si>
   <si>
-    <t>Tiempo Ejecucion</t>
-  </si>
-  <si>
-    <t>Años</t>
-  </si>
-  <si>
-    <t>Meses</t>
-  </si>
-  <si>
-    <t>Dias</t>
-  </si>
-  <si>
     <t>2 - SERVICIO</t>
   </si>
   <si>
@@ -120,9 +96,6 @@
   </si>
   <si>
     <t>DESCRIPCIÓN SERVICIO 2</t>
-  </si>
-  <si>
-    <t>0 - NO APLICA</t>
   </si>
 </sst>
 </file>
@@ -247,7 +220,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -273,18 +246,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,15 +334,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -482,24 +444,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.780612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,30 +478,12 @@
       <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -551,73 +496,30 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="H4" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="D4" s="5" t="n">
         <v>456465.45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E2:G2"/>
-  </mergeCells>
-  <dataValidations count="6">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E4" type="whole">
-      <formula1>0</formula1>
-      <formula2>1E+019</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4" type="list">
-      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12"</formula1>
-      <formula2>1E+019</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4" type="list">
-      <formula1>"0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30"</formula1>
-      <formula2>1E+019</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4" type="list">
-      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4" type="list">
       <formula1>"2 - SERVICIO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H4" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4" type="decimal">
       <formula1>0</formula1>
       <formula2>1.11111111111111E+015</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Ajuste Automatización Validaciones Cotización Ordenador Gasto
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -74,7 +74,7 @@
     <t>DESCRIPCION BIEN 2</t>
   </si>
   <si>
-    <t>5 - GRAMO</t>
+    <t>4 - KILOGRAMO</t>
   </si>
   <si>
     <t>Selección para carga de tipo Servicio</t>
@@ -334,16 +334,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,10 +416,6 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4" type="list">
-      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A4" type="list">
       <formula1>"1 - BIEN"</formula1>
       <formula2>0</formula2>
@@ -427,6 +423,10 @@
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E4" type="decimal">
       <formula1>0</formula1>
       <formula2>1.11111111111111E+015</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4" type="list">
+      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD,14 - CENTILITRO,15 - MILILITRO,16 - KILÓMETRO CUADRADO,17 - HECTÓMETRO CUADRADO,18 - DECÁMETRO CUADRADO,19 - METRO CUADRADO,20 - DECÍMETRO CUADRADO,21 - CENTÍMETRO CUADRADO,22 - MILÍMETRO CUADRADO,23 - KILÓMETRO CÚBICO,24 - HECTÓMETRO CÚBICO,25 - DECÁMETRO CÚBICO,26 - METRO CÚBICO,27 - DECÍMETRO CÚBICO,28 - CENTÍMETRO CÚBICO,29 - MILÍMETRO CÚBICO,30 - HECTÓMETRO,31 - DECÁMETRO,32 - DECÍMETRO,33 - MILÍMETRO,34 - HECTOGRAMO,35 - DECAGRAMO,36 - DECIGRAMO,37 - CENTIGRAMO,38 - MILIGRAMO,39 - KILOLITRO,40 - HECTOLITRO,41 - DECALITRO,42 - DECILITRO,"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -452,17 +452,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Ajuste Configuración Servidor de Correo Parametros en Base de Datos
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Bien" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Servicio" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="parámetros unidad" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="meses" vbProcedure="false">#REF!</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Selección para carga de tipo Bien</t>
   </si>
@@ -65,37 +66,160 @@
     <t>DESCRIPCION BIEN 1</t>
   </si>
   <si>
+    <t>35 - DECAGRAMO</t>
+  </si>
+  <si>
+    <t>BIEN 2</t>
+  </si>
+  <si>
+    <t>DESCRIPCION BIEN 2</t>
+  </si>
+  <si>
+    <t>39 - KILOLITRO</t>
+  </si>
+  <si>
+    <t>Selección para carga de tipo Servicio</t>
+  </si>
+  <si>
+    <t>Campo para nombre del Servicio</t>
+  </si>
+  <si>
+    <t>Campo para descripcion del Servicio</t>
+  </si>
+  <si>
+    <t>Campo para cantidad  del Servicio</t>
+  </si>
+  <si>
+    <t>2 - SERVICIO</t>
+  </si>
+  <si>
+    <t>SERVICIO 2</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN SERVICIO 2</t>
+  </si>
+  <si>
+    <t>0 - NO APLICA</t>
+  </si>
+  <si>
+    <t>1 - METRO</t>
+  </si>
+  <si>
+    <t>2 - KILOMETRO</t>
+  </si>
+  <si>
     <t>3 - CENTIMETRO</t>
   </si>
   <si>
-    <t>BIEN 2</t>
-  </si>
-  <si>
-    <t>DESCRIPCION BIEN 2</t>
-  </si>
-  <si>
     <t>4 - KILOGRAMO</t>
   </si>
   <si>
-    <t>Selección para carga de tipo Servicio</t>
-  </si>
-  <si>
-    <t>Campo para nombre del Servicio</t>
-  </si>
-  <si>
-    <t>Campo para descripcion del Servicio</t>
-  </si>
-  <si>
-    <t>Campo para cantidad  del Servicio</t>
-  </si>
-  <si>
-    <t>2 - SERVICIO</t>
-  </si>
-  <si>
-    <t>SERVICIO 2</t>
-  </si>
-  <si>
-    <t>DESCRIPCIÓN SERVICIO 2</t>
+    <t>5 - GRAMO</t>
+  </si>
+  <si>
+    <t>6 - MESES</t>
+  </si>
+  <si>
+    <t>7 - DIAS</t>
+  </si>
+  <si>
+    <t>8 - AÑOS</t>
+  </si>
+  <si>
+    <t>9 - SEGUNDOS</t>
+  </si>
+  <si>
+    <t>10 - MINUTOS</t>
+  </si>
+  <si>
+    <t>11 - HORAS</t>
+  </si>
+  <si>
+    <t>12 - LITRO</t>
+  </si>
+  <si>
+    <t>13 - UNIDAD</t>
+  </si>
+  <si>
+    <t>14 - CENTILITRO</t>
+  </si>
+  <si>
+    <t>15 - MILILITRO</t>
+  </si>
+  <si>
+    <t>16 - KILÓMETRO CUADRADO</t>
+  </si>
+  <si>
+    <t>17 - HECTÓMETRO CUADRADO</t>
+  </si>
+  <si>
+    <t>18 - DECÁMETRO CUADRADO</t>
+  </si>
+  <si>
+    <t>19 - METRO CUADRADO</t>
+  </si>
+  <si>
+    <t>20 - DECÍMETRO CUADRADO</t>
+  </si>
+  <si>
+    <t>21 - CENTÍMETRO CUADRADO</t>
+  </si>
+  <si>
+    <t>22 - MILÍMETRO CUADRADO</t>
+  </si>
+  <si>
+    <t>23 - KILÓMETRO CÚBICO</t>
+  </si>
+  <si>
+    <t>24 - HECTÓMETRO CÚBICO</t>
+  </si>
+  <si>
+    <t>25 - DECÁMETRO CÚBICO</t>
+  </si>
+  <si>
+    <t>26 - METRO CÚBICO</t>
+  </si>
+  <si>
+    <t>27 - DECÍMETRO CÚBICO</t>
+  </si>
+  <si>
+    <t>28 - CENTÍMETRO CÚBICO</t>
+  </si>
+  <si>
+    <t>29 - MILÍMETRO CÚBICO</t>
+  </si>
+  <si>
+    <t>30 - HECTÓMETRO</t>
+  </si>
+  <si>
+    <t>31 - DECÁMETRO</t>
+  </si>
+  <si>
+    <t>32 - DECÍMETRO</t>
+  </si>
+  <si>
+    <t>33 - MILÍMETRO</t>
+  </si>
+  <si>
+    <t>34 - HECTOGRAMO</t>
+  </si>
+  <si>
+    <t>36 - DECIGRAMO</t>
+  </si>
+  <si>
+    <t>37 - CENTIGRAMO</t>
+  </si>
+  <si>
+    <t>38 - MILIGRAMO</t>
+  </si>
+  <si>
+    <t>40 - HECTOLITRO</t>
+  </si>
+  <si>
+    <t>41 - DECALITRO</t>
+  </si>
+  <si>
+    <t>42 - DECILITRO</t>
   </si>
 </sst>
 </file>
@@ -106,7 +230,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,6 +276,20 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -169,7 +307,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF003300"/>
-        <bgColor rgb="FF333300"/>
+        <bgColor rgb="FF222222"/>
       </patternFill>
     </fill>
     <fill>
@@ -220,7 +358,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,12 +379,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -315,7 +461,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF222222"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -329,24 +475,18 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -363,7 +503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -390,10 +530,10 @@
       <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="6" t="n">
         <v>454</v>
       </c>
     </row>
@@ -410,25 +550,11 @@
       <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A3:A4" type="list">
-      <formula1>"1 - BIEN"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E3:E4" type="decimal">
-      <formula1>0</formula1>
-      <formula2>1.11111111111111E+015</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D3:D4" type="list">
-      <formula1>"0 - NO APLICA,1 - METRO,2 - KILOMETRO,3 - CENTIMETRO,4 - KILOGRAMO,5 - GRAMO,6 - MESES,7 - DIAS,8 - AÑOS,9 - SEGUNDOS,10 - MINUTOS,11 - HORAS,12 - LITRO,13 - UNIDAD,14 - CENTILITRO,15 - MILILITRO,16 - KILÓMETRO CUADRADO,17 - HECTÓMETRO CUADRADO,18 - DECÁMETRO CUADRADO,19 - METRO CUADRADO,20 - DECÍMETRO CUADRADO,21 - CENTÍMETRO CUADRADO,22 - MILÍMETRO CUADRADO,23 - KILÓMETRO CÚBICO,24 - HECTÓMETRO CÚBICO,25 - DECÁMETRO CÚBICO,26 - METRO CÚBICO,27 - DECÍMETRO CÚBICO,28 - CENTÍMETRO CÚBICO,29 - MILÍMETRO CÚBICO,30 - HECTÓMETRO,31 - DECÁMETRO,32 - DECÍMETRO,33 - MILÍMETRO,34 - HECTOGRAMO,35 - DECAGRAMO,36 - DECIGRAMO,37 - CENTIGRAMO,38 - MILIGRAMO,39 - KILOLITRO,40 - HECTOLITRO,41 - DECALITRO,42 - DECILITRO,"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -452,20 +578,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.8571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -479,13 +605,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -499,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -509,7 +635,7 @@
       <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="6" t="n">
         <v>456465.45</v>
       </c>
     </row>
@@ -532,4 +658,246 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A43"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Versión ÁGORA Sistema Desplegado (Mayo 2019)
</commit_message>
<xml_diff>
--- a/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
+++ b/blocks/gestionCotizaciones/gestionarCotizacion/plantilla/archivo_items_plantilla.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrey\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="Bien" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Servicio" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="parámetros unidad" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Bien" sheetId="1" r:id="rId1"/>
+    <sheet name="Servicio" sheetId="2" r:id="rId2"/>
+    <sheet name="parámetros unidad" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="meses" vbProcedure="false">#REF!</definedName>
+    <definedName name="meses">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -225,12 +229,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="0.00"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -239,22 +239,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
+      <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -262,7 +247,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
@@ -270,7 +255,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -318,92 +303,54 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -462,31 +409,305 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.530612244898"/>
+    <col min="1" max="2" width="10.5703125"/>
+    <col min="3" max="3" width="29.42578125"/>
+    <col min="4" max="4" width="34.140625"/>
+    <col min="5" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -520,7 +741,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -531,13 +752,13 @@
         <v>12</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="6" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6">
         <v>454</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -547,51 +768,55 @@
       <c r="C4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="6" t="n">
+      <c r="D4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="6">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'parámetros unidad'!$A$1:$A$43</xm:f>
+          </x14:formula1>
+          <xm:sqref>D3:D4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.10204081632653"/>
+    <col min="1" max="1" width="30.5703125"/>
+    <col min="2" max="2" width="26.85546875"/>
+    <col min="3" max="3" width="29.28515625"/>
+    <col min="4" max="4" width="33.85546875"/>
+    <col min="5" max="5" width="25.140625"/>
+    <col min="6" max="6" width="28.85546875"/>
+    <col min="7" max="7" width="31"/>
+    <col min="8" max="8" width="28.85546875"/>
+    <col min="9" max="9" width="24.5703125"/>
+    <col min="10" max="10" width="33.7109375"/>
+    <col min="11" max="1025" width="8.140625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -605,13 +830,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -625,7 +850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -635,269 +860,255 @@
       <c r="C4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6" t="n">
+      <c r="D4" s="6">
         <v>456465.45</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4" type="list">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A4">
       <formula1>"2 - SERVICIO"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D4" type="decimal">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="D4">
       <formula1>0</formula1>
-      <formula2>1.11111111111111E+015</formula2>
+      <formula2>1111111111111110</formula2>
     </dataValidation>
   </dataValidations>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
-    </sheetView>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.530612244898"/>
+    <col min="1" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="24.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:1" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>